<commit_message>
Test for credentials AG.
</commit_message>
<xml_diff>
--- a/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_3_test_results.xlsx
+++ b/Domibus-MSH-soapui-tests/src/main/soapui/reports/Domibus_3_2_3_test_results.xlsx
@@ -14,12 +14,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TESTS_JMS!$A$1:$K$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TESTS_WS!$A$1:$K$125</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="630">
   <si>
     <t>NEED RUNNING - 3rd/green AC enabled</t>
   </si>
@@ -1610,6 +1610,309 @@
   </si>
   <si>
     <t>Dom126-Dynamic Discovery-Needs configuration</t>
+  </si>
+  <si>
+    <t>0.342s</t>
+  </si>
+  <si>
+    <t>8.856s</t>
+  </si>
+  <si>
+    <t>2.204s</t>
+  </si>
+  <si>
+    <t>12.432s</t>
+  </si>
+  <si>
+    <t>2.207s</t>
+  </si>
+  <si>
+    <t>6.362s</t>
+  </si>
+  <si>
+    <t>4.123s</t>
+  </si>
+  <si>
+    <t>2.227s</t>
+  </si>
+  <si>
+    <t>4.088s</t>
+  </si>
+  <si>
+    <t>4.104s</t>
+  </si>
+  <si>
+    <t>4.173s</t>
+  </si>
+  <si>
+    <t>4.086s</t>
+  </si>
+  <si>
+    <t>4.082s</t>
+  </si>
+  <si>
+    <t>4.109s</t>
+  </si>
+  <si>
+    <t>4.494s</t>
+  </si>
+  <si>
+    <t>4.073s</t>
+  </si>
+  <si>
+    <t>4.075s</t>
+  </si>
+  <si>
+    <t>4.083s</t>
+  </si>
+  <si>
+    <t>4.136s</t>
+  </si>
+  <si>
+    <t>4.507s</t>
+  </si>
+  <si>
+    <t>2.236s</t>
+  </si>
+  <si>
+    <t>4.099s</t>
+  </si>
+  <si>
+    <t>4.103s</t>
+  </si>
+  <si>
+    <t>4.13s</t>
+  </si>
+  <si>
+    <t>4.061s</t>
+  </si>
+  <si>
+    <t>4.067s</t>
+  </si>
+  <si>
+    <t>4.062s</t>
+  </si>
+  <si>
+    <t>4.143s</t>
+  </si>
+  <si>
+    <t>4.074s</t>
+  </si>
+  <si>
+    <t>4.094s</t>
+  </si>
+  <si>
+    <t>4.105s</t>
+  </si>
+  <si>
+    <t>4.051s</t>
+  </si>
+  <si>
+    <t>51.98s</t>
+  </si>
+  <si>
+    <t>4.582s</t>
+  </si>
+  <si>
+    <t>0.063s</t>
+  </si>
+  <si>
+    <t>3.223s</t>
+  </si>
+  <si>
+    <t>4.364s</t>
+  </si>
+  <si>
+    <t>4.353s</t>
+  </si>
+  <si>
+    <t>0.05s</t>
+  </si>
+  <si>
+    <t>18.969s</t>
+  </si>
+  <si>
+    <t>21.797s</t>
+  </si>
+  <si>
+    <t>2.21s</t>
+  </si>
+  <si>
+    <t>2.205s</t>
+  </si>
+  <si>
+    <t>8.372s</t>
+  </si>
+  <si>
+    <t>0.358s</t>
+  </si>
+  <si>
+    <t>4.19s</t>
+  </si>
+  <si>
+    <t>0.293s</t>
+  </si>
+  <si>
+    <t>2.147s</t>
+  </si>
+  <si>
+    <t>2.138s</t>
+  </si>
+  <si>
+    <t>12.243s</t>
+  </si>
+  <si>
+    <t>2.228s</t>
+  </si>
+  <si>
+    <t>6.197s</t>
+  </si>
+  <si>
+    <t>4.05s</t>
+  </si>
+  <si>
+    <t>2.187s</t>
+  </si>
+  <si>
+    <t>4.153s</t>
+  </si>
+  <si>
+    <t>4.06s</t>
+  </si>
+  <si>
+    <t>4.076s</t>
+  </si>
+  <si>
+    <t>4.284s</t>
+  </si>
+  <si>
+    <t>4.078s</t>
+  </si>
+  <si>
+    <t>4.065s</t>
+  </si>
+  <si>
+    <t>4.038s</t>
+  </si>
+  <si>
+    <t>4.079s</t>
+  </si>
+  <si>
+    <t>4.04s</t>
+  </si>
+  <si>
+    <t>2.182s</t>
+  </si>
+  <si>
+    <t>4.044s</t>
+  </si>
+  <si>
+    <t>4.049s</t>
+  </si>
+  <si>
+    <t>4.039s</t>
+  </si>
+  <si>
+    <t>4.055s</t>
+  </si>
+  <si>
+    <t>4.035s</t>
+  </si>
+  <si>
+    <t>62.942s</t>
+  </si>
+  <si>
+    <t>4.39s</t>
+  </si>
+  <si>
+    <t>0.027s</t>
+  </si>
+  <si>
+    <t>3.173s</t>
+  </si>
+  <si>
+    <t>4.373s</t>
+  </si>
+  <si>
+    <t>0.018s</t>
+  </si>
+  <si>
+    <t>18.433s</t>
+  </si>
+  <si>
+    <t>23.577s</t>
+  </si>
+  <si>
+    <t>4.041s</t>
+  </si>
+  <si>
+    <t>2.166s</t>
+  </si>
+  <si>
+    <t>2.118s</t>
+  </si>
+  <si>
+    <t>6.873s</t>
+  </si>
+  <si>
+    <t>0.141s</t>
+  </si>
+  <si>
+    <t>4.132s</t>
+  </si>
+  <si>
+    <t>12.057s</t>
+  </si>
+  <si>
+    <t>197.424s</t>
+  </si>
+  <si>
+    <t>0.235s</t>
+  </si>
+  <si>
+    <t>0.177s</t>
+  </si>
+  <si>
+    <t>0.564s</t>
+  </si>
+  <si>
+    <t>0.162s</t>
+  </si>
+  <si>
+    <t>0.16s</t>
+  </si>
+  <si>
+    <t>0.245s</t>
+  </si>
+  <si>
+    <t>0.208s</t>
+  </si>
+  <si>
+    <t>13.287s</t>
+  </si>
+  <si>
+    <t>11.659s</t>
+  </si>
+  <si>
+    <t>Dom104-Test Experience-Truststore Update</t>
+  </si>
+  <si>
+    <t>63.526s</t>
+  </si>
+  <si>
+    <t>193.544s</t>
+  </si>
+  <si>
+    <t>101.152s</t>
+  </si>
+  <si>
+    <t>24.784s</t>
+  </si>
+  <si>
+    <t>18.131s</t>
+  </si>
+  <si>
+    <t>45.598s</t>
   </si>
 </sst>
 </file>
@@ -2787,20 +3090,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="76.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="97.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="64.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="76.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="97.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="64.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="37.5" x14ac:dyDescent="0.3">
@@ -2860,11 +3163,11 @@
       <c r="G2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="15">
-        <v>42825.50009976852</v>
+      <c r="H2" s="15" t="n">
+        <v>42829.45895636574</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>521</v>
+        <v>575</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
@@ -2899,11 +3202,11 @@
       <c r="G3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H3" s="15">
-        <v>42825.500182511576</v>
+      <c r="H3" s="15" t="n">
+        <v>42829.45896077546</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>522</v>
+        <v>576</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="13" t="s">
@@ -2938,11 +3241,11 @@
       <c r="G4" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="15">
-        <v>42821.439697048612</v>
+      <c r="H4" s="15" t="n">
+        <v>42829.4589894213</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>486</v>
+        <v>577</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
@@ -2960,7 +3263,7 @@
         <v>138</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>122</v>
+        <v>525</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>235</v>
@@ -2977,10 +3280,16 @@
       <c r="G5" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="12"/>
+      <c r="H5" s="15" t="n">
+        <v>42829.48540962963</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>612</v>
+      </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="M5" s="7" t="s">
         <v>217</v>
       </c>
@@ -2993,7 +3302,7 @@
         <v>138</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>525</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>236</v>
@@ -3010,10 +3319,16 @@
       <c r="G6" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="12"/>
+      <c r="H6" s="15" t="n">
+        <v>42829.488525671295</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>613</v>
+      </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -3073,11 +3388,11 @@
       <c r="G8" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H8" s="15">
-        <v>42821.439727743054</v>
+      <c r="H8" s="15" t="n">
+        <v>42829.45902068287</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>487</v>
+        <v>578</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
@@ -3149,11 +3464,11 @@
       <c r="G10" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H10" s="15">
-        <v>42821.439875937504</v>
+      <c r="H10" s="15" t="n">
+        <v>42829.45916824074</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>488</v>
+        <v>579</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
@@ -3218,11 +3533,11 @@
       <c r="G12" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H12" s="15">
-        <v>42821.439904942126</v>
+      <c r="H12" s="15" t="n">
+        <v>42829.45919494213</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>489</v>
+        <v>580</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
@@ -3258,11 +3573,11 @@
       <c r="G13" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H13" s="15">
-        <v>42821.439983101853</v>
+      <c r="H13" s="15" t="n">
+        <v>42829.45926934028</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>367</v>
+        <v>581</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
@@ -3298,11 +3613,11 @@
       <c r="G14" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H14" s="15">
-        <v>42821.440033599538</v>
+      <c r="H14" s="15" t="n">
+        <v>42829.459317789355</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>490</v>
+        <v>582</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
@@ -3360,11 +3675,11 @@
       <c r="G16" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="15">
-        <v>42821.440062164351</v>
+      <c r="H16" s="15" t="n">
+        <v>42829.4593453125</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>476</v>
+        <v>491</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
@@ -3393,11 +3708,11 @@
       <c r="G17" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H17" s="15">
-        <v>42821.440111585645</v>
+      <c r="H17" s="15" t="n">
+        <v>42829.459393923615</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>368</v>
+        <v>583</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
@@ -3426,11 +3741,11 @@
       <c r="G18" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="15">
-        <v>42821.440161076389</v>
+      <c r="H18" s="15" t="n">
+        <v>42829.459443391206</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>362</v>
+        <v>584</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
@@ -3517,11 +3832,11 @@
       <c r="G21" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="15">
-        <v>42821.440210636574</v>
+      <c r="H21" s="15" t="n">
+        <v>42829.45949248843</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>491</v>
+        <v>585</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
@@ -3533,7 +3848,7 @@
         <v>138</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>481</v>
+        <v>525</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>252</v>
@@ -3550,11 +3865,11 @@
       <c r="G22" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="15">
-        <v>42818.657010821757</v>
+      <c r="H22" s="15" t="n">
+        <v>42829.49107336806</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>482</v>
+        <v>614</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
@@ -3666,11 +3981,11 @@
       <c r="G26" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H26" s="15">
-        <v>42821.440259675925</v>
+      <c r="H26" s="15" t="n">
+        <v>42829.45954332176</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>363</v>
+        <v>505</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
@@ -3682,7 +3997,7 @@
         <v>138</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>481</v>
+        <v>525</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>257</v>
@@ -3699,11 +4014,11 @@
       <c r="G27" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H27" s="15">
-        <v>42818.657055023148</v>
+      <c r="H27" s="15" t="n">
+        <v>42829.49115603009</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>483</v>
+        <v>615</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
@@ -3732,11 +4047,11 @@
       <c r="G28" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H28" s="15">
-        <v>42821.440308726851</v>
+      <c r="H28" s="15" t="n">
+        <v>42829.45959144676</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>492</v>
+        <v>586</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
@@ -3806,7 +4121,7 @@
         <v>138</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>129</v>
+        <v>525</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>261</v>
@@ -3823,10 +4138,16 @@
       <c r="G31" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="12"/>
+      <c r="H31" s="15" t="n">
+        <v>42829.49125734954</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="K31" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -3850,11 +4171,11 @@
       <c r="G32" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H32" s="15">
-        <v>42821.440358472224</v>
+      <c r="H32" s="15" t="n">
+        <v>42829.45964219907</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>493</v>
+        <v>560</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1" t="s">
@@ -3883,11 +4204,11 @@
       <c r="G33" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H33" s="15">
-        <v>42821.440407754628</v>
+      <c r="H33" s="15" t="n">
+        <v>42829.45969027778</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>494</v>
+        <v>459</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
@@ -3974,11 +4295,11 @@
       <c r="G36" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H36" s="15">
-        <v>42821.440457604163</v>
+      <c r="H36" s="15" t="n">
+        <v>42829.45973864583</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>495</v>
+        <v>555</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1" t="s">
@@ -4177,11 +4498,11 @@
       <c r="G43" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H43" s="15">
-        <v>42821.44050689815</v>
+      <c r="H43" s="15" t="n">
+        <v>42829.459786921296</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>480</v>
+        <v>554</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
@@ -4295,11 +4616,11 @@
       <c r="G47" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H47" s="15">
-        <v>42821.440555706016</v>
+      <c r="H47" s="15" t="n">
+        <v>42829.45983535879</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>369</v>
+        <v>587</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1" t="s">
@@ -4328,11 +4649,11 @@
       <c r="G48" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H48" s="15">
-        <v>42821.440605335651</v>
+      <c r="H48" s="15" t="n">
+        <v>42829.45988401621</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>496</v>
+        <v>471</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1" t="s">
@@ -4419,11 +4740,11 @@
       <c r="G51" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H51" s="15">
-        <v>42821.440657418978</v>
+      <c r="H51" s="15" t="n">
+        <v>42829.45993549768</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>452</v>
+        <v>588</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1" t="s">
@@ -4510,11 +4831,11 @@
       <c r="G54" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H54" s="15">
-        <v>42821.440708564813</v>
+      <c r="H54" s="15" t="n">
+        <v>42829.45998385417</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>497</v>
+        <v>589</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1" t="s">
@@ -4526,7 +4847,7 @@
         <v>138</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>129</v>
+        <v>525</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>285</v>
@@ -4543,10 +4864,16 @@
       <c r="G55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H55" s="15"/>
-      <c r="I55" s="12"/>
+      <c r="H55" s="15" t="n">
+        <v>42829.49135383102</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>617</v>
+      </c>
       <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
+      <c r="K55" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
@@ -4570,11 +4897,11 @@
       <c r="G56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H56" s="15">
-        <v>42821.44075736111</v>
+      <c r="H56" s="15" t="n">
+        <v>42829.46003181713</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>498</v>
+        <v>590</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1" t="s">
@@ -4632,11 +4959,11 @@
       <c r="G58" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H58" s="15">
-        <v>42821.440806724539</v>
+      <c r="H58" s="15" t="n">
+        <v>42829.46008251158</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1" t="s">
@@ -4665,11 +4992,11 @@
       <c r="G59" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H59" s="15">
-        <v>42821.440855821762</v>
+      <c r="H59" s="15" t="n">
+        <v>42829.460130844906</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>500</v>
+        <v>591</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1" t="s">
@@ -4681,7 +5008,7 @@
         <v>138</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>525</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>290</v>
@@ -4698,10 +5025,16 @@
       <c r="G60" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H60" s="15"/>
-      <c r="I60" s="12"/>
+      <c r="H60" s="15" t="n">
+        <v>42829.49144326389</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>618</v>
+      </c>
       <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
+      <c r="K60" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -4725,11 +5058,11 @@
       <c r="G61" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H61" s="15">
-        <v>42821.440904699077</v>
+      <c r="H61" s="15" t="n">
+        <v>42829.46017871528</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>501</v>
+        <v>592</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1" t="s">
@@ -4816,11 +5149,11 @@
       <c r="G64" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H64" s="15">
-        <v>42821.440936631945</v>
+      <c r="H64" s="15" t="n">
+        <v>42829.4602069213</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>502</v>
+        <v>550</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1" t="s">
@@ -4878,11 +5211,11 @@
       <c r="G66" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H66" s="15">
-        <v>42821.440987662034</v>
+      <c r="H66" s="15" t="n">
+        <v>42829.46025581018</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>477</v>
+        <v>588</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1" t="s">
@@ -4911,11 +5244,11 @@
       <c r="G67" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H67" s="15">
-        <v>42821.44104503472</v>
+      <c r="H67" s="15" t="n">
+        <v>42829.46031145834</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>479</v>
+        <v>432</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1" t="s">
@@ -4944,11 +5277,11 @@
       <c r="G68" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H68" s="15">
-        <v>42821.441094490743</v>
+      <c r="H68" s="15" t="n">
+        <v>42829.460359780096</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>503</v>
+        <v>581</v>
       </c>
       <c r="J68" s="1"/>
       <c r="K68" s="1" t="s">
@@ -5006,11 +5339,11 @@
       <c r="G70" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H70" s="15">
-        <v>42821.441143356482</v>
+      <c r="H70" s="15" t="n">
+        <v>42829.46040788195</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>363</v>
+        <v>506</v>
       </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1" t="s">
@@ -5068,11 +5401,11 @@
       <c r="G72" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H72" s="15">
-        <v>42821.441192280094</v>
+      <c r="H72" s="15" t="n">
+        <v>42829.4604562963</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>480</v>
+        <v>544</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="1" t="s">
@@ -5101,11 +5434,11 @@
       <c r="G73" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H73" s="15">
-        <v>42821.441241145832</v>
+      <c r="H73" s="15" t="n">
+        <v>42829.46050474537</v>
       </c>
       <c r="I73" s="12" t="s">
-        <v>371</v>
+        <v>593</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1" t="s">
@@ -5134,11 +5467,11 @@
       <c r="G74" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H74" s="15">
-        <v>42821.441289733797</v>
+      <c r="H74" s="15" t="n">
+        <v>42829.460553240744</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>453</v>
+        <v>594</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1" t="s">
@@ -5196,11 +5529,11 @@
       <c r="G76" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H76" s="15">
-        <v>42821.441341168982</v>
+      <c r="H76" s="15" t="n">
+        <v>42829.46060414352</v>
       </c>
       <c r="I76" s="12" t="s">
-        <v>504</v>
+        <v>478</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="1" t="s">
@@ -5229,11 +5562,11 @@
       <c r="G77" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H77" s="15">
-        <v>42821.441394050926</v>
+      <c r="H77" s="15" t="n">
+        <v>42829.46065260417</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>478</v>
+        <v>595</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1" t="s">
@@ -5262,11 +5595,11 @@
       <c r="G78" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H78" s="15">
-        <v>42821.441442812502</v>
+      <c r="H78" s="15" t="n">
+        <v>42829.46070059028</v>
       </c>
       <c r="I78" s="12" t="s">
-        <v>505</v>
+        <v>596</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="1" t="s">
@@ -5295,11 +5628,11 @@
       <c r="G79" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H79" s="15">
-        <v>42821.441491620368</v>
+      <c r="H79" s="15" t="n">
+        <v>42829.46074899306</v>
       </c>
       <c r="I79" s="12" t="s">
-        <v>506</v>
+        <v>595</v>
       </c>
       <c r="J79" s="1"/>
       <c r="K79" s="1" t="s">
@@ -5311,7 +5644,7 @@
         <v>138</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>129</v>
+        <v>525</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>310</v>
@@ -5328,10 +5661,16 @@
       <c r="G80" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H80" s="15"/>
-      <c r="I80" s="12"/>
+      <c r="H80" s="15" t="n">
+        <v>42829.49165251158</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>619</v>
+      </c>
       <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
+      <c r="K80" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
@@ -5355,11 +5694,11 @@
       <c r="G81" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H81" s="15">
-        <v>42821.441540266205</v>
+      <c r="H81" s="15" t="n">
+        <v>42829.460797175925</v>
       </c>
       <c r="I81" s="12" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="J81" s="1"/>
       <c r="K81" s="1" t="s">
@@ -5388,11 +5727,11 @@
       <c r="G82" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H82" s="15">
-        <v>42821.441589652779</v>
+      <c r="H82" s="15" t="n">
+        <v>42829.46084583333</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>363</v>
+        <v>584</v>
       </c>
       <c r="J82" s="1"/>
       <c r="K82" s="1" t="s">
@@ -5421,11 +5760,11 @@
       <c r="G83" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H83" s="15">
-        <v>42821.441638888886</v>
+      <c r="H83" s="15" t="n">
+        <v>42829.46089436342</v>
       </c>
       <c r="I83" s="12" t="s">
-        <v>500</v>
+        <v>432</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1" t="s">
@@ -5437,7 +5776,7 @@
         <v>138</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>14</v>
+        <v>525</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>314</v>
@@ -5450,15 +5789,19 @@
         <v>0</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H84" s="15"/>
-      <c r="I84" s="12"/>
+        <v>136</v>
+      </c>
+      <c r="H84" s="15" t="n">
+        <v>42829.49177114583</v>
+      </c>
+      <c r="I84" s="12" t="s">
+        <v>620</v>
+      </c>
       <c r="J84" s="1" t="s">
         <v>143</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>143</v>
+        <v>356</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -5483,11 +5826,11 @@
       <c r="G85" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H85" s="15">
-        <v>42821.44168822917</v>
+      <c r="H85" s="15" t="n">
+        <v>42829.46094244213</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>361</v>
+        <v>581</v>
       </c>
       <c r="J85" s="1"/>
       <c r="K85" s="1" t="s">
@@ -5572,11 +5915,11 @@
       <c r="G88" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H88" s="15">
-        <v>42821.441737303241</v>
+      <c r="H88" s="15" t="n">
+        <v>42829.46099105324</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>500</v>
+        <v>597</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>140</v>
@@ -5607,11 +5950,11 @@
       <c r="G89" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H89" s="15">
-        <v>42821.441786006944</v>
+      <c r="H89" s="15" t="n">
+        <v>42829.4610393287</v>
       </c>
       <c r="I89" s="12" t="s">
-        <v>434</v>
+        <v>560</v>
       </c>
       <c r="J89" s="1"/>
       <c r="K89" s="1" t="s">
@@ -5669,11 +6012,11 @@
       <c r="G91" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H91" s="15">
-        <v>42821.441834317127</v>
+      <c r="H91" s="15" t="n">
+        <v>42830.40573796296</v>
       </c>
       <c r="I91" s="12" t="s">
-        <v>508</v>
+        <v>629</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1" t="s">
@@ -5702,11 +6045,11 @@
       <c r="G92" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H92" s="15">
-        <v>42821.442373124999</v>
+      <c r="H92" s="15" t="n">
+        <v>42829.46181991898</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>509</v>
+        <v>599</v>
       </c>
       <c r="J92" s="1"/>
       <c r="K92" s="1" t="s">
@@ -5735,11 +6078,11 @@
       <c r="G93" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H93" s="15">
-        <v>42821.442429085648</v>
+      <c r="H93" s="15" t="n">
+        <v>42829.46187334491</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>510</v>
+        <v>600</v>
       </c>
       <c r="J93" s="1"/>
       <c r="K93" s="1" t="s">
@@ -5797,11 +6140,11 @@
       <c r="G95" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H95" s="15">
-        <v>42821.44243048611</v>
+      <c r="H95" s="15" t="n">
+        <v>42829.46187450232</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>511</v>
+        <v>601</v>
       </c>
       <c r="J95" s="1"/>
       <c r="K95" s="1" t="s">
@@ -5830,11 +6173,11 @@
       <c r="G96" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H96" s="15">
-        <v>42821.442473009258</v>
+      <c r="H96" s="15" t="n">
+        <v>42829.46191465278</v>
       </c>
       <c r="I96" s="12" t="s">
-        <v>512</v>
+        <v>539</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1" t="s">
@@ -5863,11 +6206,11 @@
       <c r="G97" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H97" s="15">
-        <v>42821.442524918981</v>
+      <c r="H97" s="15" t="n">
+        <v>42829.461966215276</v>
       </c>
       <c r="I97" s="12" t="s">
-        <v>513</v>
+        <v>602</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="1" t="s">
@@ -5879,7 +6222,7 @@
         <v>138</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>122</v>
+        <v>525</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>328</v>
@@ -5896,10 +6239,16 @@
       <c r="G98" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H98" s="15"/>
-      <c r="I98" s="12"/>
+      <c r="H98" s="15" t="n">
+        <v>42829.49197766204</v>
+      </c>
+      <c r="I98" s="12" t="s">
+        <v>621</v>
+      </c>
       <c r="J98" s="1"/>
-      <c r="K98" s="1"/>
+      <c r="K98" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
@@ -5952,11 +6301,11 @@
       <c r="G100" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H100" s="15">
-        <v>42821.442586631943</v>
+      <c r="H100" s="15" t="n">
+        <v>42829.462020949075</v>
       </c>
       <c r="I100" s="12" t="s">
-        <v>514</v>
+        <v>603</v>
       </c>
       <c r="J100" s="1"/>
       <c r="K100" s="1" t="s">
@@ -5985,11 +6334,11 @@
       <c r="G101" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H101" s="15">
-        <v>42821.442587881946</v>
+      <c r="H101" s="15" t="n">
+        <v>42829.46202197917</v>
       </c>
       <c r="I101" s="12" t="s">
-        <v>515</v>
+        <v>604</v>
       </c>
       <c r="J101" s="1"/>
       <c r="K101" s="1" t="s">
@@ -6001,7 +6350,7 @@
         <v>138</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>122</v>
+        <v>525</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>332</v>
@@ -6018,10 +6367,16 @@
       <c r="G102" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H102" s="15"/>
-      <c r="I102" s="12"/>
+      <c r="H102" s="15" t="n">
+        <v>42829.49285243056</v>
+      </c>
+      <c r="I102" s="12" t="s">
+        <v>622</v>
+      </c>
       <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
+      <c r="K102" s="1" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
@@ -6072,11 +6427,11 @@
       <c r="G104" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H104" s="15">
-        <v>42821.442809525463</v>
+      <c r="H104" s="15" t="n">
+        <v>42829.46223856482</v>
       </c>
       <c r="I104" s="12" t="s">
-        <v>516</v>
+        <v>605</v>
       </c>
       <c r="J104" s="1"/>
       <c r="K104" s="1" t="s">
@@ -6105,11 +6460,11 @@
       <c r="G105" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H105" s="15">
-        <v>42821.443069976849</v>
+      <c r="H105" s="15" t="n">
+        <v>42829.46251508102</v>
       </c>
       <c r="I105" s="12" t="s">
-        <v>370</v>
+        <v>606</v>
       </c>
       <c r="J105" s="1"/>
       <c r="K105" s="1" t="s">
@@ -6121,13 +6476,13 @@
         <v>138</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>481</v>
+        <v>525</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>336</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>484</v>
+        <v>623</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>201</v>
@@ -6138,11 +6493,11 @@
       <c r="G106" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H106" s="15">
-        <v>42818.66925402778</v>
+      <c r="H106" s="15" t="n">
+        <v>42829.49965349537</v>
       </c>
       <c r="I106" s="12" t="s">
-        <v>485</v>
+        <v>624</v>
       </c>
       <c r="J106" s="1"/>
       <c r="K106" s="1" t="s">
@@ -6171,11 +6526,11 @@
       <c r="G107" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H107" s="15">
-        <v>42821.443119456017</v>
+      <c r="H107" s="15" t="n">
+        <v>42829.46256305555</v>
       </c>
       <c r="I107" s="12" t="s">
-        <v>517</v>
+        <v>607</v>
       </c>
       <c r="J107" s="1"/>
       <c r="K107" s="1" t="s">
@@ -6204,11 +6559,11 @@
       <c r="G108" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H108" s="15">
-        <v>42821.443150451392</v>
+      <c r="H108" s="15" t="n">
+        <v>42829.46259173611</v>
       </c>
       <c r="I108" s="12" t="s">
-        <v>518</v>
+        <v>608</v>
       </c>
       <c r="J108" s="1"/>
       <c r="K108" s="1" t="s">
@@ -6266,11 +6621,11 @@
       <c r="G110" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H110" s="15">
-        <v>42821.443177303241</v>
+      <c r="H110" s="15" t="n">
+        <v>42829.46261739583</v>
       </c>
       <c r="I110" s="12" t="s">
-        <v>519</v>
+        <v>609</v>
       </c>
       <c r="J110" s="1"/>
       <c r="K110" s="1" t="s">
@@ -6357,11 +6712,11 @@
       <c r="G113" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H113" s="15">
-        <v>42821.443267106479</v>
+      <c r="H113" s="15" t="n">
+        <v>42829.46270241898</v>
       </c>
       <c r="I113" s="12" t="s">
-        <v>520</v>
+        <v>610</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="1" t="s">
@@ -6506,11 +6861,11 @@
       <c r="G118" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H118" s="15">
-        <v>42821.443269629628</v>
+      <c r="H118" s="15" t="n">
+        <v>42829.46270517361</v>
       </c>
       <c r="I118" s="12" t="s">
-        <v>451</v>
+        <v>611</v>
       </c>
       <c r="J118" s="1"/>
       <c r="K118" s="1" t="s">
@@ -6522,7 +6877,7 @@
         <v>138</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>0</v>
+        <v>525</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>349</v>
@@ -6537,11 +6892,11 @@
       <c r="G119" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H119" s="15">
-        <v>42811.45197347222</v>
+      <c r="H119" s="15" t="n">
+        <v>42829.50085967593</v>
       </c>
       <c r="I119" s="12" t="s">
-        <v>364</v>
+        <v>625</v>
       </c>
       <c r="J119" s="1"/>
       <c r="K119" s="1" t="s">
@@ -6553,7 +6908,7 @@
         <v>138</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>0</v>
+        <v>525</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>350</v>
@@ -6568,11 +6923,11 @@
       <c r="G120" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H120" s="15">
-        <v>42811.481063391206</v>
+      <c r="H120" s="15" t="n">
+        <v>42829.503281666664</v>
       </c>
       <c r="I120" s="12" t="s">
-        <v>365</v>
+        <v>626</v>
       </c>
       <c r="J120" s="1"/>
       <c r="K120" s="1" t="s">
@@ -6584,7 +6939,7 @@
         <v>138</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>0</v>
+        <v>525</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>351</v>
@@ -6599,11 +6954,11 @@
       <c r="G121" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H121" s="15">
-        <v>42811.507301284721</v>
+      <c r="H121" s="15" t="n">
+        <v>42829.50453052083</v>
       </c>
       <c r="I121" s="12" t="s">
-        <v>366</v>
+        <v>627</v>
       </c>
       <c r="J121" s="1"/>
       <c r="K121" s="1" t="s">
@@ -6755,11 +7110,11 @@
       <c r="G127" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H127" s="15">
-        <v>42829.398912094905</v>
+      <c r="H127" s="15" t="n">
+        <v>42829.50499320602</v>
       </c>
       <c r="I127" s="12" t="s">
-        <v>527</v>
+        <v>628</v>
       </c>
       <c r="J127" s="1"/>
       <c r="K127" s="1" t="s">
@@ -6820,20 +7175,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="76.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="97.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="64.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="76.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="97.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="64.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="37.5" x14ac:dyDescent="0.3">

</xml_diff>